<commit_message>
updated deathRate=e code, recompiling
</commit_message>
<xml_diff>
--- a/03_M0+BD/Gehyra25_results_v1.xlsx
+++ b/03_M0+BD/Gehyra25_results_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/gehyra25/03_M0+BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49267A62-3CA4-C448-BDEA-8BDAD9D07BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A050E0-A6C9-8445-B53A-5699B35F1CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{A83B923C-79A0-9C49-9476-47152FCB46CC}"/>
+    <workbookView xWindow="860" yWindow="500" windowWidth="32140" windowHeight="17440" xr2:uid="{A83B923C-79A0-9C49-9476-47152FCB46CC}"/>
   </bookViews>
   <sheets>
     <sheet name="lnLs_AICs" sheetId="5" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="phybears_DECj+B=D_M0_mr3" sheetId="4" r:id="rId5"/>
     <sheet name="phybears_DEC+BD_M0_mr3" sheetId="2" r:id="rId6"/>
     <sheet name="phybears_DECj+BD_M0_mr3" sheetId="3" r:id="rId7"/>
+    <sheet name="phybears_DEC+B+D=e_M0_mr3" sheetId="8" r:id="rId8"/>
+    <sheet name="phybears_DECj+B+D=e_M0_mr3" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="102">
   <si>
     <t>rownames</t>
   </si>
@@ -342,6 +344,12 @@
   </si>
   <si>
     <t>Re-do without BGB</t>
+  </si>
+  <si>
+    <t>DEC+B+D=e M0</t>
+  </si>
+  <si>
+    <t>DEC+J+B+D=e M0</t>
   </si>
 </sst>
 </file>
@@ -403,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -420,6 +428,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A5CA8D-F4E2-2446-94D4-BA7F86E96C50}">
-  <dimension ref="B1:Q26"/>
+  <dimension ref="B1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,6 +815,12 @@
       <c r="O3" s="3" t="s">
         <v>87</v>
       </c>
+      <c r="P3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
@@ -830,6 +847,12 @@
       <c r="O4" s="5">
         <v>-334.28942280244303</v>
       </c>
+      <c r="P4">
+        <v>-340.98918313577298</v>
+      </c>
+      <c r="Q4">
+        <v>-334.31642911219802</v>
+      </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -856,6 +879,12 @@
       <c r="O5" s="5">
         <v>-9.4144064854863103</v>
       </c>
+      <c r="P5">
+        <v>-10.5043624277295</v>
+      </c>
+      <c r="Q5">
+        <v>-9.4379654086988598</v>
+      </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
@@ -906,6 +935,12 @@
       <c r="O6" s="5">
         <v>-343.70382928792901</v>
       </c>
+      <c r="P6">
+        <v>-351.49354556350198</v>
+      </c>
+      <c r="Q6">
+        <v>-343.75439452089699</v>
+      </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
@@ -950,6 +985,12 @@
       <c r="O7" s="5">
         <v>-77.006493892773804</v>
       </c>
+      <c r="P7">
+        <v>-83.232194813690498</v>
+      </c>
+      <c r="Q7">
+        <v>-77.058980252882805</v>
+      </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
@@ -993,6 +1034,12 @@
       </c>
       <c r="O8" s="5">
         <v>-77.006493892773804</v>
+      </c>
+      <c r="P8">
+        <v>-83.232194813690498</v>
+      </c>
+      <c r="Q8">
+        <v>-77.058980252882805</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.2">
@@ -1596,6 +1643,9 @@
         <f t="shared" ref="O26" si="15">O25</f>
         <v>0.15630811484031168</v>
       </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B31" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6717,4 +6767,1706 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC50CC8-3E4D-114D-8E08-7115F5EB6CAF}">
+  <dimension ref="B2:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="64.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F4">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G4">
+        <v>5.2086799486233699E-3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F5">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G5">
+        <v>3.2165896132778198E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F6">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F7">
+        <v>0.99999999999900002</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-2.5</v>
+      </c>
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-2.5</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-2.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-2.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-10</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>2.5</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F17">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>1.9999899999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>0.15489465009980199</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0.5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+      <c r="E32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F32">
+        <v>0.995</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F33">
+        <v>0.995</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <v>0.995</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB992EE8-08F6-3740-A81F-3651C3F0D769}">
+  <dimension ref="B2:I34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="73.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" s="3" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>0.01</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F4">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G4">
+        <v>1.5078988697171699E-3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F5">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G5" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F6">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F7">
+        <v>0.99999999999900002</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-2.5</v>
+      </c>
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-2.5</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-2.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-2.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>-10</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>-1</v>
+      </c>
+      <c r="F14">
+        <v>2.5</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>-1</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F17">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="G17">
+        <v>7.9722735385734707E-3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>2.9920277264614201</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19">
+        <v>1.9999899999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>1.99468515097428</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.997342575487142</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.997342575487142</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.997342575487142</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>0.16273455591858499</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1E-4</v>
+      </c>
+      <c r="F26">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0.5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>0.1</v>
+      </c>
+      <c r="E32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F32">
+        <v>0.995</v>
+      </c>
+      <c r="G32">
+        <v>0.1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F33">
+        <v>0.995</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <v>0.995</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update - 12 models
</commit_message>
<xml_diff>
--- a/03_M0+BD/Gehyra25_results_v1.xlsx
+++ b/03_M0+BD/Gehyra25_results_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/gehyra25/03_M0+BD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A050E0-A6C9-8445-B53A-5699B35F1CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C32676E-8467-7D41-953B-AF69EA18A093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="500" windowWidth="32140" windowHeight="17440" xr2:uid="{A83B923C-79A0-9C49-9476-47152FCB46CC}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <sheet name="phybears_DECj+BD_M0_mr3" sheetId="3" r:id="rId7"/>
     <sheet name="phybears_DEC+B+D=e_M0_mr3" sheetId="8" r:id="rId8"/>
     <sheet name="phybears_DECj+B+D=e_M0_mr3" sheetId="9" r:id="rId9"/>
+    <sheet name="phybears_DEC+B=D=e_M0_mr3" sheetId="10" r:id="rId10"/>
+    <sheet name="phybears_DECj+B=D=e_M0_mr3" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="104">
   <si>
     <t>rownames</t>
   </si>
@@ -351,6 +353,12 @@
   <si>
     <t>DEC+J+B+D=e M0</t>
   </si>
+  <si>
+    <t>DEC+B=D=e_M0_mr3</t>
+  </si>
+  <si>
+    <t>DEC++J+B=D=e_M0_mr3</t>
+  </si>
 </sst>
 </file>
 
@@ -411,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A5CA8D-F4E2-2446-94D4-BA7F86E96C50}">
-  <dimension ref="B1:Q31"/>
+  <dimension ref="B1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -778,7 +787,7 @@
     <col min="10" max="15" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D1" s="2" t="s">
         <v>88</v>
       </c>
@@ -786,7 +795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="D3" s="3" t="s">
         <v>82</v>
       </c>
@@ -821,8 +830,14 @@
       <c r="Q3" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>76</v>
       </c>
@@ -848,13 +863,13 @@
         <v>-334.28942280244303</v>
       </c>
       <c r="P4">
-        <v>-340.98918313577298</v>
+        <v>-340.28260604883599</v>
       </c>
       <c r="Q4">
-        <v>-334.31642911219802</v>
-      </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+        <v>-334.635835955689</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>78</v>
       </c>
@@ -880,13 +895,13 @@
         <v>-9.4144064854863103</v>
       </c>
       <c r="P5">
-        <v>-10.5043624277295</v>
+        <v>-10.7709745718255</v>
       </c>
       <c r="Q5">
-        <v>-9.4379654086988598</v>
-      </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+        <v>-9.3485911447979309</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>79</v>
       </c>
@@ -936,13 +951,13 @@
         <v>-343.70382928792901</v>
       </c>
       <c r="P6">
-        <v>-351.49354556350198</v>
+        <v>-351.05358062066102</v>
       </c>
       <c r="Q6">
-        <v>-343.75439452089699</v>
-      </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+        <v>-343.98442710048698</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>80</v>
       </c>
@@ -986,13 +1001,13 @@
         <v>-77.006493892773804</v>
       </c>
       <c r="P7">
-        <v>-83.232194813690498</v>
+        <v>-83.563531884234905</v>
       </c>
       <c r="Q7">
-        <v>-77.058980252882805</v>
-      </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+        <v>-77.319326827283703</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>81</v>
       </c>
@@ -1036,73 +1051,85 @@
         <v>-77.006493892773804</v>
       </c>
       <c r="P8">
-        <v>-83.232194813690498</v>
+        <v>-83.563531884234905</v>
       </c>
       <c r="Q8">
-        <v>-77.058980252882805</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+        <v>-77.319326827283703</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>90</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>96</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>96</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>96</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="5">
         <v>96</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>96</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <v>96</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="5">
         <v>96</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="5">
         <v>96</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="5">
         <v>96</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="5">
         <v>96</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="5">
         <v>96</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P10" s="5">
+        <v>96</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>96</v>
+      </c>
+      <c r="R10" s="5">
+        <v>96</v>
+      </c>
+      <c r="S10" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>91</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>4</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>3</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>3</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>4</v>
       </c>
       <c r="J11" s="5">
@@ -1123,8 +1150,20 @@
       <c r="O11" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P11" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>4</v>
+      </c>
+      <c r="R11" s="5">
+        <v>2</v>
+      </c>
+      <c r="S11" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>92</v>
       </c>
@@ -1176,68 +1215,84 @@
         <f>-2*(O6)+(2*O11*O10/(O10-O11-1))</f>
         <v>698.07432524252465</v>
       </c>
-      <c r="P12" t="s">
+      <c r="P12">
+        <f>-2*(P6)+(2*P11*P10/(P10-P11-1))</f>
+        <v>708.36803080653942</v>
+      </c>
+      <c r="Q12">
+        <f>-2*(Q6)+(2*Q11*Q10/(Q10-Q11-1))</f>
+        <v>696.40841464053437</v>
+      </c>
+      <c r="T12" t="s">
         <v>94</v>
       </c>
-      <c r="Q12">
-        <f>MIN(D12:O12)</f>
+      <c r="U12">
+        <f>MIN(D12:Q12)</f>
         <v>695.92473131412441</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>93</v>
       </c>
       <c r="D13">
-        <f>D12-$Q$12</f>
+        <f>D12-$U$12</f>
         <v>12.397605703311228</v>
       </c>
       <c r="E13">
-        <f>E12-$Q$12</f>
+        <f>E12-$U$12</f>
         <v>0.34089944443303466</v>
       </c>
       <c r="F13">
-        <f>F12-$Q$12</f>
+        <f>F12-$U$12</f>
         <v>21.577605703311178</v>
       </c>
       <c r="G13">
-        <f>G12-$Q$12</f>
+        <f>G12-$U$12</f>
         <v>12.86089944443313</v>
       </c>
       <c r="H13">
-        <f>H12-$Q$12</f>
+        <f>H12-$U$12</f>
         <v>77.317605703311187</v>
       </c>
       <c r="I13">
-        <f>I12-$Q$12</f>
+        <f>I12-$U$12</f>
         <v>27.340899444433035</v>
       </c>
       <c r="J13">
-        <f>J12-$Q$12</f>
+        <f>J12-$U$12</f>
         <v>12.413166816466969</v>
       </c>
       <c r="K13">
-        <f>K12-$Q$12</f>
+        <f>K12-$U$12</f>
         <v>0.3490117450839989</v>
       </c>
       <c r="L13">
-        <f>L12-$Q$12</f>
+        <f>L12-$U$12</f>
         <v>53.356075457865018</v>
       </c>
       <c r="M13">
-        <f>M12-$Q$12</f>
+        <f>M12-$U$12</f>
         <v>0</v>
       </c>
       <c r="N13">
-        <f>N12-$Q$12</f>
+        <f>N12-$U$12</f>
         <v>14.581563964287966</v>
       </c>
       <c r="O13">
-        <f>O12-$Q$12</f>
+        <f>O12-$U$12</f>
         <v>2.1495939284002361</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P13">
+        <f>P12-$U$12</f>
+        <v>12.443299492415008</v>
+      </c>
+      <c r="Q13">
+        <f>Q12-$U$12</f>
+        <v>0.48368332640995959</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>95</v>
       </c>
@@ -1289,131 +1344,155 @@
         <f t="shared" si="0"/>
         <v>0.34136705799896538</v>
       </c>
-      <c r="P14" t="s">
+      <c r="P14">
+        <f t="shared" ref="P14" si="1">EXP(-0.5*P13)</f>
+        <v>1.9859661730512669E-3</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ref="Q14" si="2">EXP(-0.5*Q13)</f>
+        <v>0.78518049067230467</v>
+      </c>
+      <c r="T14" t="s">
         <v>96</v>
       </c>
-      <c r="Q14">
-        <f>SUM(D14:O14)</f>
-        <v>3.0308877485390449</v>
-      </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <f>SUM(D14:Q14)</f>
+        <v>3.8180542053844007</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>97</v>
       </c>
       <c r="D15">
-        <f>D14/$Q$14</f>
-        <v>6.7038497933007981E-4</v>
+        <f>D14/$U$14</f>
+        <v>5.3217202044714617E-4</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:O15" si="1">E14/$Q$14</f>
-        <v>0.27823052420677591</v>
+        <f>E14/$U$14</f>
+        <v>0.22086786664753794</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>6.8063237507728857E-6</v>
+        <f>F14/$U$14</f>
+        <v>5.4030671538700474E-6</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
-        <v>5.3176691988507038E-4</v>
+        <f>G14/$U$14</f>
+        <v>4.2213278174130464E-4</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
-        <v>5.3595137855205389E-18</v>
+        <f>H14/$U$14</f>
+        <v>4.2545453251428814E-18</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>3.8144266527068636E-7</v>
+        <f>I14/$U$14</f>
+        <v>3.0280080867071039E-7</v>
       </c>
       <c r="J15">
-        <f t="shared" si="1"/>
-        <v>6.6518925011317014E-4</v>
+        <f>J14/$U$14</f>
+        <v>5.2804749230240438E-4</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
-        <v>0.27710426505779662</v>
+        <f>K14/$U$14</f>
+        <v>0.21997380782262463</v>
       </c>
       <c r="L15">
-        <f t="shared" si="1"/>
-        <v>8.5566855841894643E-13</v>
+        <f>L14/$U$14</f>
+        <v>6.7925577035146999E-13</v>
       </c>
       <c r="M15">
-        <f t="shared" si="1"/>
-        <v>0.32993633646842324</v>
+        <f>M14/$U$14</f>
+        <v>0.2619135156828713</v>
       </c>
       <c r="N15">
-        <f t="shared" si="1"/>
-        <v>2.2494884322176454E-4</v>
+        <f>N14/$U$14</f>
+        <v>1.7857124500940226E-4</v>
       </c>
       <c r="O15">
-        <f t="shared" si="1"/>
-        <v>0.11262939650718239</v>
-      </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+        <f>O14/$U$14</f>
+        <v>8.9408646298827665E-2</v>
+      </c>
+      <c r="P15">
+        <f>P14/$U$14</f>
+        <v>5.2015138241111498E-4</v>
+      </c>
+      <c r="Q15">
+        <f>Q14/$U$14</f>
+        <v>0.20564938275758526</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>98</v>
       </c>
       <c r="D16" s="7">
         <f>D15</f>
-        <v>6.7038497933007981E-4</v>
+        <v>5.3217202044714617E-4</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" ref="E16:O16" si="2">E15</f>
-        <v>0.27823052420677591</v>
+        <f t="shared" ref="E16:O16" si="3">E15</f>
+        <v>0.22086786664753794</v>
       </c>
       <c r="F16" s="7">
-        <f t="shared" si="2"/>
-        <v>6.8063237507728857E-6</v>
+        <f t="shared" si="3"/>
+        <v>5.4030671538700474E-6</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3176691988507038E-4</v>
+        <f t="shared" si="3"/>
+        <v>4.2213278174130464E-4</v>
       </c>
       <c r="H16" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3595137855205389E-18</v>
+        <f t="shared" si="3"/>
+        <v>4.2545453251428814E-18</v>
       </c>
       <c r="I16" s="7">
-        <f t="shared" si="2"/>
-        <v>3.8144266527068636E-7</v>
+        <f t="shared" si="3"/>
+        <v>3.0280080867071039E-7</v>
       </c>
       <c r="J16" s="7">
-        <f t="shared" si="2"/>
-        <v>6.6518925011317014E-4</v>
+        <f t="shared" si="3"/>
+        <v>5.2804749230240438E-4</v>
       </c>
       <c r="K16" s="7">
-        <f t="shared" si="2"/>
-        <v>0.27710426505779662</v>
+        <f t="shared" si="3"/>
+        <v>0.21997380782262463</v>
       </c>
       <c r="L16" s="7">
-        <f t="shared" si="2"/>
-        <v>8.5566855841894643E-13</v>
+        <f t="shared" si="3"/>
+        <v>6.7925577035146999E-13</v>
       </c>
       <c r="M16" s="7">
-        <f t="shared" si="2"/>
-        <v>0.32993633646842324</v>
+        <f t="shared" si="3"/>
+        <v>0.2619135156828713</v>
       </c>
       <c r="N16" s="7">
-        <f t="shared" si="2"/>
-        <v>2.2494884322176454E-4</v>
+        <f t="shared" si="3"/>
+        <v>1.7857124500940226E-4</v>
       </c>
       <c r="O16" s="7">
-        <f t="shared" si="2"/>
-        <v>0.11262939650718239</v>
-      </c>
-    </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>8.9408646298827665E-2</v>
+      </c>
+      <c r="P16" s="7">
+        <f t="shared" ref="P16" si="4">P15</f>
+        <v>5.2015138241111498E-4</v>
+      </c>
+      <c r="Q16" s="7">
+        <f t="shared" ref="Q16" si="5">Q15</f>
+        <v>0.20564938275758526</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>99</v>
       </c>
       <c r="H18" s="1"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
       <c r="J19" s="3" t="s">
         <v>82</v>
       </c>
@@ -1432,31 +1511,55 @@
       <c r="O19" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>90</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="5">
         <v>96</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="5">
         <v>96</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="5">
         <v>96</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="5">
         <v>96</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="5">
         <v>96</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="5">
         <v>96</v>
       </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P20" s="5">
+        <v>96</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>96</v>
+      </c>
+      <c r="R20" s="5">
+        <v>96</v>
+      </c>
+      <c r="S20" s="5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>91</v>
       </c>
@@ -1478,8 +1581,20 @@
       <c r="O21" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P21" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>4</v>
+      </c>
+      <c r="R21" s="5">
+        <v>2</v>
+      </c>
+      <c r="S21" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>92</v>
       </c>
@@ -1488,128 +1603,160 @@
         <v>708.33789813059138</v>
       </c>
       <c r="K22">
-        <f t="shared" ref="K22:O22" si="3">-2*(K6)+(2*K21*K20/(K20-K21-1))</f>
+        <f t="shared" ref="K22:O22" si="6">-2*(K6)+(2*K21*K20/(K20-K21-1))</f>
         <v>696.27374305920841</v>
       </c>
       <c r="L22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>749.28080677198943</v>
       </c>
       <c r="M22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>695.92473131412441</v>
       </c>
       <c r="N22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>710.50629527841238</v>
       </c>
       <c r="O22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>698.07432524252465</v>
       </c>
-      <c r="P22" t="s">
+      <c r="P22">
+        <f t="shared" ref="P22" si="7">-2*(P6)+(2*P21*P20/(P20-P21-1))</f>
+        <v>708.36803080653942</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ref="Q22" si="8">-2*(Q6)+(2*Q21*Q20/(Q20-Q21-1))</f>
+        <v>696.40841464053437</v>
+      </c>
+      <c r="T22" t="s">
         <v>94</v>
       </c>
-      <c r="Q22">
-        <f>MIN(J22:O22)</f>
+      <c r="U22">
+        <f>MIN(J22:Q22)</f>
         <v>695.92473131412441</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>93</v>
       </c>
       <c r="J23">
-        <f>J22-$Q$22</f>
+        <f>J22-$U$22</f>
         <v>12.413166816466969</v>
       </c>
       <c r="K23">
-        <f>K22-$Q$12</f>
+        <f>K22-$U$12</f>
         <v>0.3490117450839989</v>
       </c>
       <c r="L23">
-        <f>L22-$Q$12</f>
+        <f>L22-$U$12</f>
         <v>53.356075457865018</v>
       </c>
       <c r="M23">
-        <f>M22-$Q$12</f>
+        <f>M22-$U$12</f>
         <v>0</v>
       </c>
       <c r="N23">
-        <f>N22-$Q$12</f>
+        <f>N22-$U$12</f>
         <v>14.581563964287966</v>
       </c>
       <c r="O23">
-        <f>O22-$Q$12</f>
+        <f>O22-$U$12</f>
         <v>2.1495939284002361</v>
       </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P23">
+        <f>P22-$U$12</f>
+        <v>12.443299492415008</v>
+      </c>
+      <c r="Q23">
+        <f>Q22-$U$12</f>
+        <v>0.48368332640995959</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>95</v>
       </c>
       <c r="J24">
-        <f t="shared" ref="J24" si="4">EXP(-0.5*J23)</f>
+        <f t="shared" ref="J24" si="9">EXP(-0.5*J23)</f>
         <v>2.0161139486278819E-3</v>
       </c>
       <c r="K24">
-        <f t="shared" ref="K24" si="5">EXP(-0.5*K23)</f>
+        <f t="shared" ref="K24" si="10">EXP(-0.5*K23)</f>
         <v>0.83987192203159189</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24" si="6">EXP(-0.5*L23)</f>
+        <f t="shared" ref="L24" si="11">EXP(-0.5*L23)</f>
         <v>2.5934353505220508E-12</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24" si="7">EXP(-0.5*M23)</f>
+        <f t="shared" ref="M24" si="12">EXP(-0.5*M23)</f>
         <v>1</v>
       </c>
       <c r="N24">
-        <f t="shared" ref="N24" si="8">EXP(-0.5*N23)</f>
+        <f t="shared" ref="N24" si="13">EXP(-0.5*N23)</f>
         <v>6.8179469296887651E-4</v>
       </c>
       <c r="O24">
-        <f t="shared" ref="O24" si="9">EXP(-0.5*O23)</f>
+        <f t="shared" ref="O24" si="14">EXP(-0.5*O23)</f>
         <v>0.34136705799896538</v>
       </c>
-      <c r="P24" t="s">
+      <c r="P24">
+        <f t="shared" ref="P24" si="15">EXP(-0.5*P23)</f>
+        <v>1.9859661730512669E-3</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ref="Q24" si="16">EXP(-0.5*Q23)</f>
+        <v>0.78518049067230467</v>
+      </c>
+      <c r="T24" t="s">
         <v>96</v>
       </c>
-      <c r="Q24">
-        <f>SUM(J24:O24)</f>
-        <v>2.1839368886747472</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="U24">
+        <f>SUM(J24:Q24)</f>
+        <v>2.971103345520103</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>97</v>
       </c>
       <c r="J25">
-        <f>J24/$Q$24</f>
-        <v>9.2315577390667946E-4</v>
+        <f>J24/$U$24</f>
+        <v>6.7857415719578529E-4</v>
       </c>
       <c r="K25">
-        <f t="shared" ref="K25:O25" si="10">K24/$Q$24</f>
-        <v>0.38456785376304603</v>
+        <f>K24/$U$24</f>
+        <v>0.28268014416192216</v>
       </c>
       <c r="L25">
-        <f t="shared" si="10"/>
-        <v>1.1875047140651554E-12</v>
+        <f>L24/$U$24</f>
+        <v>8.7288628126399281E-13</v>
       </c>
       <c r="M25">
-        <f t="shared" si="10"/>
-        <v>0.45788868954304729</v>
+        <f>M24/$U$24</f>
+        <v>0.33657530005067737</v>
       </c>
       <c r="N25">
-        <f t="shared" si="10"/>
-        <v>3.1218607850092315E-4</v>
+        <f>N24/$U$24</f>
+        <v>2.2947525335895906E-4</v>
       </c>
       <c r="O25">
-        <f t="shared" si="10"/>
-        <v>0.15630811484031168</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+        <f>O24/$U$24</f>
+        <v>0.11489571997341876</v>
+      </c>
+      <c r="P25">
+        <f>P24/$U$24</f>
+        <v>6.6842716058522565E-4</v>
+      </c>
+      <c r="Q25">
+        <f>Q24/$U$24</f>
+        <v>0.26427235924196901</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>98</v>
       </c>
@@ -1621,35 +1768,1792 @@
       <c r="I26" s="7"/>
       <c r="J26" s="7">
         <f>J25</f>
-        <v>9.2315577390667946E-4</v>
+        <v>6.7857415719578529E-4</v>
       </c>
       <c r="K26" s="7">
-        <f t="shared" ref="K26" si="11">K25</f>
-        <v>0.38456785376304603</v>
+        <f t="shared" ref="K26" si="17">K25</f>
+        <v>0.28268014416192216</v>
       </c>
       <c r="L26" s="7">
-        <f t="shared" ref="L26" si="12">L25</f>
-        <v>1.1875047140651554E-12</v>
+        <f t="shared" ref="L26" si="18">L25</f>
+        <v>8.7288628126399281E-13</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" ref="M26" si="13">M25</f>
-        <v>0.45788868954304729</v>
+        <f t="shared" ref="M26" si="19">M25</f>
+        <v>0.33657530005067737</v>
       </c>
       <c r="N26" s="7">
-        <f t="shared" ref="N26" si="14">N25</f>
-        <v>3.1218607850092315E-4</v>
+        <f t="shared" ref="N26" si="20">N25</f>
+        <v>2.2947525335895906E-4</v>
       </c>
       <c r="O26" s="7">
-        <f t="shared" ref="O26" si="15">O25</f>
-        <v>0.15630811484031168</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
+        <f t="shared" ref="O26" si="21">O25</f>
+        <v>0.11489571997341876</v>
+      </c>
+      <c r="P26" s="7">
+        <f t="shared" ref="P26" si="22">P25</f>
+        <v>6.6842716058522565E-4</v>
+      </c>
+      <c r="Q26" s="7">
+        <f t="shared" ref="Q26" si="23">Q25</f>
+        <v>0.26427235924196901</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32">
+        <v>-340.28260604883599</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33">
+        <v>-10.7709745718255</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34">
+        <v>-351.05358062066102</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35">
+        <v>-83.563531884234905</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36">
+        <v>-83.563531884234905</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DC02F3-EA09-B040-A139-39503B0A9248}">
+  <dimension ref="B4:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:I36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F5">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G5">
+        <v>7.4500715927155901E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F6">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G6">
+        <v>0.21489196213054701</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F7">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F8">
+        <v>0.99999999999900002</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-2.5</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-2.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-2.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-2.5</v>
+      </c>
+      <c r="F12">
+        <v>2.5</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>-10</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>-10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>-100</v>
+      </c>
+      <c r="E15">
+        <v>-100</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>-100</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>2.5</v>
+      </c>
+      <c r="G17">
+        <v>-100</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
+        <v>1.9999899999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>0.21489196213054701</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0.21489196213054701</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G32">
+        <v>0.5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>0.1</v>
+      </c>
+      <c r="E33">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F33">
+        <v>0.995</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <v>0.995</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F35">
+        <v>0.995</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>66</v>
+      </c>
+      <c r="I35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{457EF7F3-4E69-A146-BB65-4E080B730F75}">
+  <dimension ref="B4:I35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F5">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G5">
+        <v>5.8724341181914698E-3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F6">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G6">
+        <v>0.10847155900397901</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F7">
+        <v>4.9999999999989999</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>9.9999999999999998E-13</v>
+      </c>
+      <c r="F8">
+        <v>0.99999999999900002</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-2.5</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-2.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-2.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-2.5</v>
+      </c>
+      <c r="F12">
+        <v>2.5</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>-10</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>-10</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>-100</v>
+      </c>
+      <c r="E15">
+        <v>-100</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>-100</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>-1</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>-1</v>
+      </c>
+      <c r="F17">
+        <v>2.5</v>
+      </c>
+      <c r="G17">
+        <v>-100</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F18">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="G18">
+        <v>2.97233773489573E-3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19">
+        <v>2.9999899999999999</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>2.9970276622651002</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20">
+        <v>1.9999899999999999</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>1.9980184415100599</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0.99900922075503396</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.99900922075503396</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+      <c r="I22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.99900922075503396</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>0.10847155900397901</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25">
+        <v>0.165369597267503</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
+        <v>0.10847155900397901</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1E-4</v>
+      </c>
+      <c r="F27">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1E-4</v>
+      </c>
+      <c r="F28">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1E-4</v>
+      </c>
+      <c r="F29">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>10</v>
+      </c>
+      <c r="I29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1E-4</v>
+      </c>
+      <c r="F30">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1E-4</v>
+      </c>
+      <c r="F31">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>1E-4</v>
+      </c>
+      <c r="F32">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="G32">
+        <v>0.5</v>
+      </c>
+      <c r="H32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>0.1</v>
+      </c>
+      <c r="E33">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F33">
+        <v>0.995</v>
+      </c>
+      <c r="G33">
+        <v>0.1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F34">
+        <v>0.995</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>66</v>
+      </c>
+      <c r="I34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F35">
+        <v>0.995</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>66</v>
+      </c>
+      <c r="I35" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1658,7 +3562,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="A1:XFD1048576"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3360,7 +5264,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="A1:XFD1048576"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6774,7 +8678,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7625,7 +9529,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7677,7 +9581,7 @@
         <v>4.9999999999989999</v>
       </c>
       <c r="G4">
-        <v>1.5078988697171699E-3</v>
+        <v>1.46079694863598E-3</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
@@ -7702,8 +9606,8 @@
       <c r="F5">
         <v>4.9999999999989999</v>
       </c>
-      <c r="G5" s="1">
-        <v>9.9999999999999998E-13</v>
+      <c r="G5" s="9">
+        <v>1.2925393929450299E-3</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
@@ -7928,7 +9832,7 @@
         <v>15</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="E14">
         <v>-1</v>
@@ -7937,7 +9841,7 @@
         <v>2.5</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
@@ -7963,7 +9867,7 @@
         <v>2.5</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="H15" t="s">
         <v>10</v>
@@ -7989,7 +9893,7 @@
         <v>2.5</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>-100</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
@@ -8015,7 +9919,7 @@
         <v>2.9999899999999999</v>
       </c>
       <c r="G17">
-        <v>7.9722735385734707E-3</v>
+        <v>7.7982224237437697E-3</v>
       </c>
       <c r="H17" t="s">
         <v>10</v>
@@ -8041,7 +9945,7 @@
         <v>3</v>
       </c>
       <c r="G18">
-        <v>2.9920277264614201</v>
+        <v>2.9922017775762502</v>
       </c>
       <c r="H18" t="s">
         <v>10</v>
@@ -8067,7 +9971,7 @@
         <v>2</v>
       </c>
       <c r="G19">
-        <v>1.99468515097428</v>
+        <v>1.99480118505083</v>
       </c>
       <c r="H19" t="s">
         <v>10</v>
@@ -8093,7 +9997,7 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.997342575487142</v>
+        <v>0.99740059252541802</v>
       </c>
       <c r="H20" t="s">
         <v>10</v>
@@ -8119,7 +10023,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <v>0.997342575487142</v>
+        <v>0.99740059252541802</v>
       </c>
       <c r="H21" t="s">
         <v>10</v>
@@ -8145,7 +10049,7 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0.997342575487142</v>
+        <v>0.99740059252541802</v>
       </c>
       <c r="H22" t="s">
         <v>10</v>
@@ -8171,7 +10075,7 @@
         <v>2</v>
       </c>
       <c r="G23">
-        <v>0.16273455591858499</v>
+        <v>0.17880390743734001</v>
       </c>
       <c r="H23" t="s">
         <v>10</v>
@@ -8197,7 +10101,7 @@
         <v>2</v>
       </c>
       <c r="G24">
-        <v>6.9999999999999999E-4</v>
+        <v>1.2925393929450299E-3</v>
       </c>
       <c r="H24" t="s">
         <v>10</v>

</xml_diff>